<commit_message>
Added README.md with example code.
</commit_message>
<xml_diff>
--- a/ReleaseCheckSheet_0.2.1.xlsx
+++ b/ReleaseCheckSheet_0.2.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>MDACSHTTPServer Release Checkoff</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Was version properly marked in NUGET configuration before commit?</t>
+  </si>
+  <si>
+    <t>Has version in project configuration and NUGET config been updated?</t>
   </si>
 </sst>
 </file>
@@ -117,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -126,6 +132,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B14" sqref="B14:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +501,10 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="4" t="str">
+        <f>"514716e1"</f>
+        <v>514716e1</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -641,9 +653,43 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
     <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="B15:J15"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>

</xml_diff>

<commit_message>
Added README.md. Added release check off for 0.2.1
</commit_message>
<xml_diff>
--- a/ReleaseCheckSheet_0.2.1.xlsx
+++ b/ReleaseCheckSheet_0.2.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>MDACSHTTPServer Release Checkoff</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Was version properly marked in NUGET configuration before commit?</t>
+  </si>
+  <si>
+    <t>Has version in project configuration and NUGET config been updated?</t>
   </si>
 </sst>
 </file>
@@ -117,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -126,6 +132,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B14" sqref="B14:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +501,10 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="4" t="str">
+        <f>"514716e1"</f>
+        <v>514716e1</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -641,9 +653,43 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
     <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="B15:J15"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>

</xml_diff>